<commit_message>
a few changes after DLS course June 2019
</commit_message>
<xml_diff>
--- a/Python3/src/18 Financial Python/Spreadsheets/data/writingToCells.xlsx
+++ b/Python3/src/18 Financial Python/Spreadsheets/data/writingToCells.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="writing to cells" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="writing to cells" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="9">
   <si>
     <t>--A--</t>
   </si>
@@ -46,23 +51,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="dd-mm-yyyy" numFmtId="165"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -78,16 +82,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -375,324 +380,321 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="1" t="n">
-        <v>42853.61634723916</v>
-      </c>
-      <c r="B1" t="n">
+      <c r="A1" s="1">
+        <v>43629.657488812532</v>
+      </c>
+      <c r="B1">
         <v>42</v>
       </c>
-      <c r="C1" t="n">
+      <c r="C1">
         <v>43</v>
       </c>
-      <c r="D1" t="n">
+      <c r="D1">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" t="n">
+      <c r="A2">
         <v>25</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>28</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>31</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>34</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>37</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>40</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>43</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>46</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>49</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2">
         <v>52</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2">
         <v>55</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2">
         <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" t="n">
+      <c r="A3">
         <v>25</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>28</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>31</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>34</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>37</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>40</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>43</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>46</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3">
         <v>49</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J3">
         <v>52</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3">
         <v>55</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" t="n">
+      <c r="A4">
         <v>25</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>28</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>31</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>34</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>37</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>40</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>43</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>46</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4">
         <v>49</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J4">
         <v>52</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K4">
         <v>55</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L4">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" t="n">
+      <c r="A5">
         <v>25</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>28</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>31</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>34</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>37</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>40</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>43</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5">
         <v>46</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5">
         <v>49</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J5">
         <v>52</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K5">
         <v>55</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L5">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" t="n">
+      <c r="A6">
         <v>25</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>28</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>31</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>34</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>37</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>40</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>43</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>46</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6">
         <v>49</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J6">
         <v>52</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K6">
         <v>55</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L6">
         <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="B7" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="E7">
         <v>25</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>64</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K7">
         <v>121</v>
       </c>
-      <c r="N7" t="n">
+      <c r="N7">
         <v>196</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="Q7">
         <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="B8" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" t="n">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="E8">
         <v>25</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8">
         <v>64</v>
       </c>
-      <c r="K8" t="n">
+      <c r="K8">
         <v>121</v>
       </c>
-      <c r="N8" t="n">
+      <c r="N8">
         <v>196</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="Q8">
         <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="B9" t="n">
-        <v>4</v>
-      </c>
-      <c r="E9" t="n">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="E9">
         <v>25</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9">
         <v>64</v>
       </c>
-      <c r="K9" t="n">
+      <c r="K9">
         <v>121</v>
       </c>
-      <c r="N9" t="n">
+      <c r="N9">
         <v>196</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="Q9">
         <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="B10" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" t="n">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="E10">
         <v>25</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10">
         <v>64</v>
       </c>
-      <c r="K10" t="n">
+      <c r="K10">
         <v>121</v>
       </c>
-      <c r="N10" t="n">
+      <c r="N10">
         <v>196</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="Q10">
         <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="B11" t="n">
-        <v>4</v>
-      </c>
-      <c r="E11" t="n">
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="E11">
         <v>25</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11">
         <v>64</v>
       </c>
-      <c r="K11" t="n">
+      <c r="K11">
         <v>121</v>
       </c>
-      <c r="N11" t="n">
+      <c r="N11">
         <v>196</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="Q11">
         <v>289</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -721,7 +723,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -750,7 +752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -779,7 +781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -808,7 +810,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -837,7 +839,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -866,7 +868,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -895,7 +897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -924,7 +926,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -953,7 +955,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -983,6 +985,11 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>